<commit_message>
minor formating and updates
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,102 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Candy</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.599594973848947e+18</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>6/3/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>chip</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.599594973848947e+18</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>6/3/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Biscuit</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.599594973848947e+18</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6/3/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Banana</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.599594973848947e+18</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>6/3/2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>